<commit_message>
read for version 1.1.2, crowdsupply build
</commit_message>
<xml_diff>
--- a/pcb/R1001_BOM.xlsx
+++ b/pcb/R1001_BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="105">
   <si>
     <t>Reference</t>
   </si>
@@ -125,7 +125,7 @@
     <t>100 nF</t>
   </si>
   <si>
-    <t>C14 C9 </t>
+    <t>C112 C14 C9 </t>
   </si>
   <si>
     <t>CC0603KRX5R6BB105</t>
@@ -140,28 +140,13 @@
     <t>X5R</t>
   </si>
   <si>
-    <t>J1 </t>
-  </si>
-  <si>
-    <t>PCIEXPRESS-X1</t>
-  </si>
-  <si>
-    <t>Main:PCIEXPRESS-X1</t>
-  </si>
-  <si>
-    <t>Amphenol FCI</t>
-  </si>
-  <si>
-    <t>10018784-10200TLF</t>
-  </si>
-  <si>
     <t>J2 </t>
   </si>
   <si>
     <t>CONN_01X04</t>
   </si>
   <si>
-    <t>Main:SOCKET254P-01X04</t>
+    <t>Main:70553-0038</t>
   </si>
   <si>
     <t>Molex</t>
@@ -200,6 +185,24 @@
     <t>2N7002P,215</t>
   </si>
   <si>
+    <t>R120 R121 </t>
+  </si>
+  <si>
+    <t>RC0603FR-07100KL</t>
+  </si>
+  <si>
+    <t>Main:RESC0603</t>
+  </si>
+  <si>
+    <t>±1%</t>
+  </si>
+  <si>
+    <t>100 kΩ</t>
+  </si>
+  <si>
+    <t>100 mW</t>
+  </si>
+  <si>
     <t>R15 </t>
   </si>
   <si>
@@ -212,31 +215,22 @@
     <t>Panasonic Electronic Components</t>
   </si>
   <si>
-    <t>±1%</t>
-  </si>
-  <si>
     <t>0.05 Ω</t>
   </si>
   <si>
     <t>1W</t>
   </si>
   <si>
-    <t>R18 </t>
+    <t>R18 R4 </t>
   </si>
   <si>
     <t>RC0603FR-072K8L</t>
   </si>
   <si>
-    <t>Main:RESC0603</t>
-  </si>
-  <si>
     <t>2.80 kΩ</t>
   </si>
   <si>
-    <t>100 mW</t>
-  </si>
-  <si>
-    <t>R1 R10 R11 R12 R13 R14 R16 R17 R2 R21 R4 R6 R7 </t>
+    <t>R1 R10 R11 R12 R13 R14 R16 R17 R2 R6 R7 </t>
   </si>
   <si>
     <t>RC0603FR-0710KL</t>
@@ -245,15 +239,6 @@
     <t>10.0 kΩ</t>
   </si>
   <si>
-    <t>R20 </t>
-  </si>
-  <si>
-    <t>RC0603FR-0715KL</t>
-  </si>
-  <si>
-    <t>15.0 kΩ</t>
-  </si>
-  <si>
     <t>R3 </t>
   </si>
   <si>
@@ -323,7 +308,7 @@
     <t>U3 </t>
   </si>
   <si>
-    <t>EFM8BB10F2G</t>
+    <t>EFM8BB10F8G</t>
   </si>
   <si>
     <t>Main:QFN50P300X300X75-20NT170X170</t>
@@ -332,7 +317,7 @@
     <t>Silicon Labs</t>
   </si>
   <si>
-    <t>EFM8BB10F2G-A-QFN20R</t>
+    <t>EFM8BB10F8G-A-QFN20R</t>
   </si>
   <si>
     <t>U4 </t>
@@ -440,15 +425,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.9387755102041"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.37755102040816"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3316326530612"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3061224489796"/>
@@ -619,7 +604,7 @@
         <v>36</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>37</v>
@@ -677,7 +662,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>47</v>
@@ -692,7 +677,7 @@
         <v>50</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,7 +685,7 @@
         <v>51</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>52</v>
@@ -715,7 +700,7 @@
         <v>55</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,7 +708,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>57</v>
@@ -732,39 +717,48 @@
         <v>58</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>28</v>
       </c>
+      <c r="J9" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="M10" s="0" t="s">
         <v>66</v>
@@ -778,13 +772,13 @@
         <v>68</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>69</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>17</v>
@@ -796,173 +790,164 @@
         <v>18</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>17</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="G15" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="M15" s="0" t="s">
         <v>84</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="N16" s="0" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,38 +1007,15 @@
         <v>102</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="G19" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>105</v>
-      </c>
       <c r="H19" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" s="0" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>